<commit_message>
changed data file for driver analytics
</commit_message>
<xml_diff>
--- a/config/analytics.xlsx
+++ b/config/analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2d171d6dd3c2b1f/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D07AD3AE-C1BB-4982-ABA8-1A624C43FFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{D07AD3AE-C1BB-4982-ABA8-1A624C43FFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D1565B49-E47D-4E68-BEA4-B9D5D5C50AD9}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{B651C5F8-289B-4F4F-8CE1-D1C4B8DB47BC}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -502,7 +502,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="5">
-        <v>247.5</v>
+        <v>270</v>
       </c>
       <c r="C2">
         <v>250</v>
@@ -512,7 +512,7 @@
       </c>
       <c r="E2" s="5">
         <f>B2-C2</f>
-        <v>-2.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -520,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="5">
-        <v>323.39999999999998</v>
+        <v>262</v>
       </c>
       <c r="C3">
         <v>330</v>
@@ -530,7 +530,7 @@
       </c>
       <c r="E3" s="5">
         <f t="shared" ref="E3:E13" si="0">B3-C3</f>
-        <v>-6.6000000000000227</v>
+        <v>-68</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -538,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5">
-        <v>204.6</v>
+        <v>283</v>
       </c>
       <c r="C4">
         <v>250</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>-45.400000000000006</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -556,7 +556,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="5">
-        <v>193.20000000000002</v>
+        <v>291</v>
       </c>
       <c r="C5">
         <v>210</v>
@@ -566,7 +566,7 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>-16.799999999999983</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -574,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="5">
-        <v>169.2</v>
+        <v>295</v>
       </c>
       <c r="C6">
         <v>180</v>
@@ -584,7 +584,7 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>-10.800000000000011</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -592,7 +592,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="5">
-        <v>167.2</v>
+        <v>285</v>
       </c>
       <c r="C7">
         <v>190</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>-22.800000000000011</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -610,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="5">
-        <v>149.6</v>
+        <v>275</v>
       </c>
       <c r="C8">
         <v>170</v>
@@ -620,7 +620,7 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>-20.400000000000006</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -628,7 +628,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="5">
-        <v>139.19999999999999</v>
+        <v>299</v>
       </c>
       <c r="C9">
         <v>160</v>
@@ -638,7 +638,7 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>-20.800000000000011</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -646,7 +646,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="5">
-        <v>143.55000000000001</v>
+        <v>283</v>
       </c>
       <c r="C10">
         <v>155</v>
@@ -656,7 +656,7 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" si="0"/>
-        <v>-11.449999999999989</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -664,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="5">
-        <v>154.80000000000001</v>
+        <v>298</v>
       </c>
       <c r="C11">
         <v>144</v>
@@ -674,7 +674,7 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>
-        <v>10.800000000000011</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -682,7 +682,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="5">
-        <v>177</v>
+        <v>292</v>
       </c>
       <c r="C12">
         <v>130</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="F12" s="6"/>
     </row>
@@ -701,7 +701,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="5">
-        <v>187</v>
+        <v>289</v>
       </c>
       <c r="C13">
         <v>120</v>
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed wording of analytics
</commit_message>
<xml_diff>
--- a/config/analytics.xlsx
+++ b/config/analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2d171d6dd3c2b1f/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{D07AD3AE-C1BB-4982-ABA8-1A624C43FFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D1565B49-E47D-4E68-BEA4-B9D5D5C50AD9}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{D07AD3AE-C1BB-4982-ABA8-1A624C43FFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4AD9D577-6477-43CE-BDE0-5761745DA3BF}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{B651C5F8-289B-4F4F-8CE1-D1C4B8DB47BC}"/>
   </bookViews>
@@ -139,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -151,9 +151,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -472,7 +479,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -501,217 +508,217 @@
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
-        <v>270</v>
-      </c>
-      <c r="C2">
-        <v>250</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="6">
+        <v>67.5</v>
+      </c>
+      <c r="C2" s="6">
+        <v>62.5</v>
+      </c>
+      <c r="D2" s="7">
         <v>40</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <f>B2-C2</f>
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
-        <v>262</v>
-      </c>
-      <c r="C3">
-        <v>330</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="6">
+        <v>83</v>
+      </c>
+      <c r="C3" s="6">
+        <v>82.5</v>
+      </c>
+      <c r="D3" s="7">
         <v>38</v>
       </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E13" si="0">B3-C3</f>
-        <v>-68</v>
+      <c r="E3" s="6">
+        <f>B3-C3</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
-        <v>283</v>
-      </c>
-      <c r="C4">
-        <v>250</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="6">
+        <v>70.75</v>
+      </c>
+      <c r="C4" s="6">
+        <v>62.5</v>
+      </c>
+      <c r="D4" s="7">
         <v>30</v>
       </c>
-      <c r="E4" s="5">
-        <f t="shared" si="0"/>
-        <v>33</v>
+      <c r="E4" s="6">
+        <f>B4-C4</f>
+        <v>8.25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
-        <v>291</v>
-      </c>
-      <c r="C5">
-        <v>210</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="6">
+        <v>72.75</v>
+      </c>
+      <c r="C5" s="6">
+        <v>52.5</v>
+      </c>
+      <c r="D5" s="7">
         <v>27</v>
       </c>
-      <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>81</v>
+      <c r="E5" s="6">
+        <f>B5-C5</f>
+        <v>20.25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
-        <v>295</v>
-      </c>
-      <c r="C6">
-        <v>180</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="6">
+        <v>73.75</v>
+      </c>
+      <c r="C6" s="6">
+        <v>45</v>
+      </c>
+      <c r="D6" s="7">
         <v>25</v>
       </c>
-      <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>115</v>
+      <c r="E6" s="6">
+        <f>B6-C6</f>
+        <v>28.75</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5">
-        <v>285</v>
-      </c>
-      <c r="C7">
-        <v>190</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="6">
+        <v>71.25</v>
+      </c>
+      <c r="C7" s="6">
+        <v>47.5</v>
+      </c>
+      <c r="D7" s="7">
         <v>24</v>
       </c>
-      <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>95</v>
+      <c r="E7" s="6">
+        <f>B7-C7</f>
+        <v>23.75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
-        <v>275</v>
-      </c>
-      <c r="C8">
-        <v>170</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="6">
+        <v>68.75</v>
+      </c>
+      <c r="C8" s="6">
+        <v>42.5</v>
+      </c>
+      <c r="D8" s="7">
         <v>24</v>
       </c>
-      <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>105</v>
+      <c r="E8" s="6">
+        <f>B8-C8</f>
+        <v>26.25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5">
-        <v>299</v>
-      </c>
-      <c r="C9">
-        <v>160</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="6">
+        <v>74.75</v>
+      </c>
+      <c r="C9" s="6">
+        <v>40</v>
+      </c>
+      <c r="D9" s="7">
         <v>23</v>
       </c>
-      <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>139</v>
+      <c r="E9" s="6">
+        <f>B9-C9</f>
+        <v>34.75</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
-        <v>283</v>
-      </c>
-      <c r="C10">
-        <v>155</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="6">
+        <v>70.75</v>
+      </c>
+      <c r="C10" s="6">
+        <v>38.75</v>
+      </c>
+      <c r="D10" s="7">
         <v>21</v>
       </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>128</v>
+      <c r="E10" s="6">
+        <f>B10-C10</f>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5">
-        <v>298</v>
-      </c>
-      <c r="C11">
-        <v>144</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="6">
+        <v>74.5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7">
         <v>20</v>
       </c>
-      <c r="E11" s="5">
-        <f t="shared" si="0"/>
-        <v>154</v>
+      <c r="E11" s="6">
+        <f>B11-C11</f>
+        <v>38.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5">
-        <v>292</v>
-      </c>
-      <c r="C12">
-        <v>130</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="6">
+        <v>73</v>
+      </c>
+      <c r="C12" s="6">
+        <v>32.5</v>
+      </c>
+      <c r="D12" s="7">
         <v>18</v>
       </c>
-      <c r="E12" s="7">
-        <f t="shared" si="0"/>
-        <v>162</v>
-      </c>
-      <c r="F12" s="6"/>
+      <c r="E12" s="8">
+        <f>B12-C12</f>
+        <v>40.5</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5">
-        <v>289</v>
-      </c>
-      <c r="C13">
-        <v>120</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="6">
+        <v>72.25</v>
+      </c>
+      <c r="C13" s="6">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7">
         <v>17</v>
       </c>
-      <c r="E13" s="5">
-        <f t="shared" si="0"/>
-        <v>169</v>
+      <c r="E13" s="6">
+        <f>B13-C13</f>
+        <v>42.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed decimal on analytics page
</commit_message>
<xml_diff>
--- a/config/analytics.xlsx
+++ b/config/analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2d171d6dd3c2b1f/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{D07AD3AE-C1BB-4982-ABA8-1A624C43FFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4AD9D577-6477-43CE-BDE0-5761745DA3BF}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{D07AD3AE-C1BB-4982-ABA8-1A624C43FFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4EBAA30B-7191-48F0-A45C-486BBD5B4A3F}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{B651C5F8-289B-4F4F-8CE1-D1C4B8DB47BC}"/>
   </bookViews>
@@ -91,8 +91,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -139,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,7 +159,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -479,7 +483,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -517,8 +521,8 @@
       <c r="D2" s="7">
         <v>40</v>
       </c>
-      <c r="E2" s="6">
-        <f>B2-C2</f>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E13" si="0">B2-C2</f>
         <v>5</v>
       </c>
     </row>
@@ -535,8 +539,8 @@
       <c r="D3" s="7">
         <v>38</v>
       </c>
-      <c r="E3" s="6">
-        <f>B3-C3</f>
+      <c r="E3" s="8">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -553,8 +557,8 @@
       <c r="D4" s="7">
         <v>30</v>
       </c>
-      <c r="E4" s="6">
-        <f>B4-C4</f>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
         <v>8.25</v>
       </c>
     </row>
@@ -571,8 +575,8 @@
       <c r="D5" s="7">
         <v>27</v>
       </c>
-      <c r="E5" s="6">
-        <f>B5-C5</f>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
         <v>20.25</v>
       </c>
     </row>
@@ -589,8 +593,8 @@
       <c r="D6" s="7">
         <v>25</v>
       </c>
-      <c r="E6" s="6">
-        <f>B6-C6</f>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
         <v>28.75</v>
       </c>
     </row>
@@ -607,8 +611,8 @@
       <c r="D7" s="7">
         <v>24</v>
       </c>
-      <c r="E7" s="6">
-        <f>B7-C7</f>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
         <v>23.75</v>
       </c>
     </row>
@@ -625,8 +629,8 @@
       <c r="D8" s="7">
         <v>24</v>
       </c>
-      <c r="E8" s="6">
-        <f>B8-C8</f>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
         <v>26.25</v>
       </c>
     </row>
@@ -643,8 +647,8 @@
       <c r="D9" s="7">
         <v>23</v>
       </c>
-      <c r="E9" s="6">
-        <f>B9-C9</f>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
         <v>34.75</v>
       </c>
     </row>
@@ -661,8 +665,8 @@
       <c r="D10" s="7">
         <v>21</v>
       </c>
-      <c r="E10" s="6">
-        <f>B10-C10</f>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
@@ -679,8 +683,8 @@
       <c r="D11" s="7">
         <v>20</v>
       </c>
-      <c r="E11" s="6">
-        <f>B11-C11</f>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
         <v>38.5</v>
       </c>
     </row>
@@ -688,18 +692,18 @@
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>73</v>
       </c>
-      <c r="C12" s="6">
-        <v>32.5</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="C12" s="8">
+        <v>32</v>
+      </c>
+      <c r="D12" s="8">
         <v>18</v>
       </c>
-      <c r="E12" s="8">
-        <f>B12-C12</f>
-        <v>40.5</v>
+      <c r="E12" s="9">
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -716,8 +720,8 @@
       <c r="D13" s="7">
         <v>17</v>
       </c>
-      <c r="E13" s="6">
-        <f>B13-C13</f>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
         <v>42.25</v>
       </c>
     </row>

</xml_diff>